<commit_message>
Added OpenXmlEmbedObjectNew project to embed documents into compliance form - word
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_Test_InvalidValues.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_Test_InvalidValues.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Address</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>ggn</t>
+  </si>
+  <si>
+    <t>"3211/3441"</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <dimension ref="A1:BF14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,9 +611,7 @@
       <c r="C2" s="5">
         <v>8522</v>
       </c>
-      <c r="D2" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
@@ -656,9 +657,7 @@
       <c r="C3" s="5">
         <v>8522</v>
       </c>
-      <c r="D3" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
@@ -683,9 +682,7 @@
       <c r="C4" s="5">
         <v>8522</v>
       </c>
-      <c r="D4" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
@@ -708,9 +705,7 @@
       <c r="C5" s="5">
         <v>8522</v>
       </c>
-      <c r="D5" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
@@ -733,9 +728,7 @@
       <c r="C6" s="5">
         <v>8522</v>
       </c>
-      <c r="D6" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
@@ -758,9 +751,7 @@
       <c r="C7" s="5">
         <v>8522</v>
       </c>
-      <c r="D7" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
@@ -783,11 +774,9 @@
       <c r="C8" s="5">
         <v>8522</v>
       </c>
-      <c r="D8" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="2"/>
@@ -808,9 +797,7 @@
       <c r="C9" s="5">
         <v>8522</v>
       </c>
-      <c r="D9" s="2">
-        <v>34234</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="5" t="s">
         <v>24</v>
       </c>

</xml_diff>